<commit_message>
fungsi export history transaksi aktif
</commit_message>
<xml_diff>
--- a/public/master_part_number.xlsx
+++ b/public/master_part_number.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
   <si>
     <t>Part Number</t>
   </si>
@@ -24,6 +24,12 @@
   </si>
   <si>
     <t>Maximum Kapasitas</t>
+  </si>
+  <si>
+    <t>4111-03550-C</t>
+  </si>
+  <si>
+    <t>Besar</t>
   </si>
 </sst>
 </file>
@@ -363,7 +369,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -380,6 +386,28 @@
       </c>
       <c r="C1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>